<commit_message>
classification tag at UI for ml and fuzzy added
</commit_message>
<xml_diff>
--- a/data/business_exception.xlsx
+++ b/data/business_exception.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Exception</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Invite not found in both CBS mailbox</t>
+  </si>
+  <si>
+    <t>Apple Inc. is an American multinational technology company that specializes in consumer electronics, computer software, and online services. Apple is the world's largest technology company by revenue and, since January 2021, the world's most valuable company. Wikipedia</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -457,6 +460,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>